<commit_message>
adding code from rpi
</commit_message>
<xml_diff>
--- a/docs/ARM_Cortex_A53_64Bit_QuadCore.xlsx
+++ b/docs/ARM_Cortex_A53_64Bit_QuadCore.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
   <si>
     <t xml:space="preserve">CPU Clockcycles were gathered with the perf linux utility as the testing was done on a Raspberry Pi</t>
   </si>
   <si>
-    <t xml:space="preserve">Float</t>
+    <t xml:space="preserve">Float Sine</t>
   </si>
   <si>
     <t xml:space="preserve">Run 1</t>
@@ -64,7 +64,19 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Double</t>
+    <t xml:space="preserve">Float Bearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float ReEntry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Sine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Bearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double ReEntry</t>
   </si>
 </sst>
 </file>
@@ -74,11 +86,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -94,12 +107,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -155,11 +162,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,21 +187,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -273,84 +287,398 @@
         <v>3263208.4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="L6" s="0" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3030795</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>3017176</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>3031169</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3299788</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3022229</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>3016718</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>3294832</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>3324933</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>3032888</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>3295863</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">SUM(B7:K7)/10</f>
+        <v>3136639.1</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B10" s="0" t="n">
+        <v>3353063</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3053322</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>3057435</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>3345958</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>3054958</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>3066966</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>3325634</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>3058163</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>3343855</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>3059787</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">SUM(B10:K10)/10</f>
+        <v>3171914.1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <v>3221994</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C13" s="0" t="n">
         <v>3224567</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>3518944</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>3224445</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>3235711</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>3534564</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>3212685</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>3218594</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>3218321</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K13" s="0" t="n">
         <v>3535102</v>
       </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">SUM(B8:K8)/10</f>
+      <c r="L13" s="0" t="n">
+        <f aca="false">SUM(B13:K13)/10</f>
         <v>3314492.7</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3021029</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>3008361</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>3305040</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>3319347</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>3289463</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>3285000</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>3302215</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>3027615</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>3297377</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>3025186</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">SUM(B16:K16)/10</f>
+        <v>3188063.3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3328379</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3058241</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>3189262</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>3349459</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>3061389</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>3076501</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>3099893</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>3058812</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>3333319</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>3060463</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">SUM(B19:K19)/10</f>
+        <v>3161571.8</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>